<commit_message>
main changed to depende only on GPT-API
</commit_message>
<xml_diff>
--- a/files/Table_Structure_Template.xlsx
+++ b/files/Table_Structure_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wjahn\OneDrive\VSCODE Workbench\Python\pbi_sqlsolver\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\Projects\gpt_bi\pbi_sqlsolver\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1979F98-CA35-4D80-BB94-071491CC0A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB98BC4D-B0DC-4959-A051-E5D813F68BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -508,13 +508,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -546,7 +546,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -561,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -574,7 +574,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -587,7 +587,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -602,7 +602,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -617,7 +617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -630,7 +630,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -643,7 +643,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -658,7 +658,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -673,7 +673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -699,7 +699,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -716,7 +716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -733,7 +733,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -748,7 +748,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -761,7 +761,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -789,7 +789,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -815,7 +815,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -830,7 +830,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -843,7 +843,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -856,7 +856,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -869,7 +869,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
@@ -886,7 +886,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -903,7 +903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -916,7 +916,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
@@ -931,7 +931,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -957,7 +957,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -974,7 +974,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -991,7 +991,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1004,7 +1004,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>